<commit_message>
Finished Arduino Firmware, updated/added a lot of documentation for setup, debugging/troubleshooting and usage
</commit_message>
<xml_diff>
--- a/Pneumatic System Bill of Materials.xlsx
+++ b/Pneumatic System Bill of Materials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RJ\Documents\.Rowan Fall 2018\Consultant\OpenSourcePneumaticSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51FE560-D5D1-4063-8DBC-36CB14D8B17A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D613FEF-DA84-4B99-ADE0-EF4D3411DE3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="33120" windowHeight="22656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Quantity</t>
   </si>
@@ -162,15 +163,25 @@
   </si>
   <si>
     <t>Similar DC power source can be used if cheaper one is found. Also, 12V can be used. This source was on hand during development and therefore used for development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least one breadboard and a couple jumper wires are needed for the circuitry. This pack has more than needed but is cheaper than other packs that have only the amount of resources needed  https://www.amazon.com/eBoot-400-Point-Solderless-Breadboard-Flexible/dp/B071D7V9HD/ref=sr_1_5?ie=UTF8&amp;qid=1544299357&amp;sr=8-5&amp;keywords=breadboard+and+wires </t>
+  </si>
+  <si>
+    <t>eBoot 3 Pieces 400-Point Solderless Circuit Breadboard with 65 Pieces M/M Flexible Breadboard Jumper Wires</t>
+  </si>
+  <si>
+    <t>eBoot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="00000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -276,7 +287,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -321,6 +332,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -643,10 +657,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="8">
-        <f t="shared" ref="G3:G11" si="0">F3*E3</f>
+        <f t="shared" ref="G3:G12" si="0">F3*E3</f>
         <v>398</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -796,161 +810,185 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="13">
-        <f>SUM(G2:G5)</f>
-        <v>471.37</v>
-      </c>
-      <c r="H6" s="5"/>
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="16">
+        <v>712971918559</v>
+      </c>
+      <c r="E6" s="8">
+        <v>8.99</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>8.99</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="13">
+        <f>SUM(G2:G6)</f>
+        <v>480.36</v>
+      </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D9" s="5">
         <v>90150</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E9" s="15">
         <v>29.93</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F9" s="5">
         <v>2</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G9" s="8">
         <f t="shared" si="0"/>
         <v>59.86</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E10" s="8">
         <v>485</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G10" s="8">
         <f t="shared" si="0"/>
         <v>485</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E11" s="15">
         <v>29.95</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F11" s="5">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G11" s="8">
         <f t="shared" si="0"/>
         <v>29.95</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E12" s="8">
         <v>6.69</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G12" s="8">
         <f t="shared" si="0"/>
         <v>20.07</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="12" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="13">
-        <f>SUM(G6,G8:G11)</f>
-        <v>1066.25</v>
-      </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G13" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="G13" s="13">
+        <f>SUM(G7,G9:G12)</f>
+        <v>1075.24</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
@@ -963,14 +1001,17 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>

</xml_diff>